<commit_message>
Added requirement that every instruction has been followed by every other instruction called Instr Mix
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/SimulationVerificationPlan/base_instruction_set/CV32E40P_RV32I_Base_Instructions.xlsx
+++ b/verif/CV32E40P/SimulationVerificationPlan/base_instruction_set/CV32E40P_RV32I_Base_Instructions.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mike\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\gtumbush\mcu\GTumbush\core-v-docs\update_rv32i_dvplan\verif\CV32E40P\SimulationVerificationPlan\base_instruction_set\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DB622AD-D351-4183-8991-7A8E8C29F274}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RV32I" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -30,17 +29,26 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>tc={CB605BA4-E843-417A-93C2-ADE20C9EA930}</author>
   </authors>
   <commentList>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{CB605BA4-E843-417A-93C2-ADE20C9EA930}">
+    <comment ref="J1" authorId="0" shapeId="0">
       <text>
-        <t>[Threaded comment]
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     In a refactoring of the uvmt_cv32 environment, the functional coverage for all RV32 ISA instructions has been moved from class_coverage.svh to cv32/env/uvme_cv32/cov/uvme_rv32isa_covg.sv</t>
+        </r>
       </text>
     </comment>
   </commentList>
@@ -48,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="219">
   <si>
     <t>Requirement Location</t>
   </si>
@@ -1331,12 +1339,28 @@
   <si>
     <t>Note: the "HINT" instructions (rd == 0) have been stricken from this Vplan because they are redundant.  The rd == 0 condition is already covered above.</t>
   </si>
+  <si>
+    <t>Instr mix</t>
+  </si>
+  <si>
+    <t>All instructions have been followed by every other instruction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercise instruction such that every instruction has been followed by every other instruction.
+</t>
+  </si>
+  <si>
+    <t>Cross last instruction executed with current instruction executed.</t>
+  </si>
+  <si>
+    <t>uvme_rv32isa_covg.sv.instr_cg.cr_ins_prev_x_ins</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1383,12 +1407,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1441,7 +1459,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1476,16 +1494,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1506,11 +1518,23 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1907,10 +1931,13 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F37D5184-1C62-497B-8D21-1B81168DE377}">
-  <dimension ref="B1:AMC67"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B1:AMC68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A45" sqref="A45"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1931,7 +1958,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:12" s="3" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="22" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
@@ -1991,10 +2018,10 @@
       </c>
     </row>
     <row r="3" spans="2:12" ht="83.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="15" t="s">
+      <c r="C3" s="24" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="9" t="s">
@@ -2026,8 +2053,8 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B4" s="15"/>
-      <c r="C4" s="15"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="24"/>
       <c r="D4" s="9" t="s">
         <v>19</v>
       </c>
@@ -2057,8 +2084,8 @@
       </c>
     </row>
     <row r="5" spans="2:12" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B5" s="15"/>
-      <c r="C5" s="15"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="24"/>
       <c r="D5" s="9" t="s">
         <v>22</v>
       </c>
@@ -2088,8 +2115,8 @@
       </c>
     </row>
     <row r="6" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
       <c r="D6" s="9" t="s">
         <v>24</v>
       </c>
@@ -2119,8 +2146,8 @@
       </c>
     </row>
     <row r="7" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="9" t="s">
         <v>26</v>
       </c>
@@ -2150,8 +2177,8 @@
       </c>
     </row>
     <row r="8" spans="2:12" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="9" t="s">
         <v>28</v>
       </c>
@@ -2181,8 +2208,8 @@
       </c>
     </row>
     <row r="9" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
+      <c r="B9" s="24"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="9" t="s">
         <v>31</v>
       </c>
@@ -2212,8 +2239,8 @@
       </c>
     </row>
     <row r="10" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
+      <c r="B10" s="24"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="9" t="s">
         <v>34</v>
       </c>
@@ -2243,8 +2270,8 @@
       </c>
     </row>
     <row r="11" spans="2:12" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="9" t="s">
         <v>36</v>
       </c>
@@ -2274,8 +2301,8 @@
       </c>
     </row>
     <row r="12" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="9" t="s">
         <v>39</v>
       </c>
@@ -2305,8 +2332,8 @@
       </c>
     </row>
     <row r="13" spans="2:12" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="9" t="s">
         <v>41</v>
       </c>
@@ -2336,10 +2363,10 @@
       </c>
     </row>
     <row r="14" spans="2:12" ht="56.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="24" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="24" t="s">
         <v>45</v>
       </c>
       <c r="D14" s="9" t="s">
@@ -2351,13 +2378,13 @@
       <c r="F14" s="12" t="s">
         <v>186</v>
       </c>
-      <c r="G14" s="16" t="s">
+      <c r="G14" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="H14" s="16" t="s">
+      <c r="H14" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="I14" s="16" t="s">
+      <c r="I14" s="27" t="s">
         <v>21</v>
       </c>
       <c r="J14" s="10" t="s">
@@ -2371,8 +2398,8 @@
       </c>
     </row>
     <row r="15" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
+      <c r="B15" s="24"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="9" t="s">
         <v>48</v>
       </c>
@@ -2382,9 +2409,9 @@
       <c r="F15" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
+      <c r="G15" s="27"/>
+      <c r="H15" s="27"/>
+      <c r="I15" s="27"/>
       <c r="J15" s="10" t="s">
         <v>196</v>
       </c>
@@ -2396,8 +2423,8 @@
       </c>
     </row>
     <row r="16" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B16" s="15"/>
-      <c r="C16" s="15"/>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
       <c r="D16" s="9" t="s">
         <v>49</v>
       </c>
@@ -2407,9 +2434,9 @@
       <c r="F16" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
+      <c r="G16" s="27"/>
+      <c r="H16" s="27"/>
+      <c r="I16" s="27"/>
       <c r="J16" s="10" t="s">
         <v>199</v>
       </c>
@@ -2421,8 +2448,8 @@
       </c>
     </row>
     <row r="17" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B17" s="15"/>
-      <c r="C17" s="15"/>
+      <c r="B17" s="24"/>
+      <c r="C17" s="24"/>
       <c r="D17" s="9" t="s">
         <v>51</v>
       </c>
@@ -2432,9 +2459,9 @@
       <c r="F17" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G17" s="16"/>
-      <c r="H17" s="16"/>
-      <c r="I17" s="16"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
       <c r="J17" s="10" t="s">
         <v>152</v>
       </c>
@@ -2446,8 +2473,8 @@
       </c>
     </row>
     <row r="18" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
+      <c r="B18" s="24"/>
+      <c r="C18" s="24"/>
       <c r="D18" s="9" t="s">
         <v>53</v>
       </c>
@@ -2457,9 +2484,9 @@
       <c r="F18" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="16"/>
+      <c r="G18" s="27"/>
+      <c r="H18" s="27"/>
+      <c r="I18" s="27"/>
       <c r="J18" s="10" t="s">
         <v>191</v>
       </c>
@@ -2471,8 +2498,8 @@
       </c>
     </row>
     <row r="19" spans="2:12" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
       <c r="D19" s="9" t="s">
         <v>55</v>
       </c>
@@ -2482,9 +2509,9 @@
       <c r="F19" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="16"/>
+      <c r="G19" s="27"/>
+      <c r="H19" s="27"/>
+      <c r="I19" s="27"/>
       <c r="J19" s="10" t="s">
         <v>208</v>
       </c>
@@ -2496,8 +2523,8 @@
       </c>
     </row>
     <row r="20" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B20" s="15"/>
-      <c r="C20" s="15"/>
+      <c r="B20" s="24"/>
+      <c r="C20" s="24"/>
       <c r="D20" s="9" t="s">
         <v>58</v>
       </c>
@@ -2507,9 +2534,9 @@
       <c r="F20" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="16"/>
+      <c r="G20" s="27"/>
+      <c r="H20" s="27"/>
+      <c r="I20" s="27"/>
       <c r="J20" s="10" t="s">
         <v>193</v>
       </c>
@@ -2521,8 +2548,8 @@
       </c>
     </row>
     <row r="21" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
+      <c r="B21" s="24"/>
+      <c r="C21" s="24"/>
       <c r="D21" s="9" t="s">
         <v>60</v>
       </c>
@@ -2532,9 +2559,9 @@
       <c r="F21" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="16"/>
+      <c r="G21" s="27"/>
+      <c r="H21" s="27"/>
+      <c r="I21" s="27"/>
       <c r="J21" s="10" t="s">
         <v>204</v>
       </c>
@@ -2546,8 +2573,8 @@
       </c>
     </row>
     <row r="22" spans="2:12" ht="94.5" x14ac:dyDescent="0.25">
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="24"/>
       <c r="D22" s="9" t="s">
         <v>62</v>
       </c>
@@ -2557,9 +2584,9 @@
       <c r="F22" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="16"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
       <c r="J22" s="10" t="s">
         <v>202</v>
       </c>
@@ -2571,8 +2598,8 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="78.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="15"/>
-      <c r="C23" s="15"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
       <c r="D23" s="9" t="s">
         <v>65</v>
       </c>
@@ -2582,9 +2609,9 @@
       <c r="F23" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="16"/>
+      <c r="G23" s="27"/>
+      <c r="H23" s="27"/>
+      <c r="I23" s="27"/>
       <c r="J23" s="10" t="s">
         <v>205</v>
       </c>
@@ -2596,8 +2623,8 @@
       </c>
     </row>
     <row r="24" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24"/>
       <c r="D24" s="9" t="s">
         <v>68</v>
       </c>
@@ -2624,10 +2651,10 @@
       </c>
     </row>
     <row r="25" spans="2:12" ht="114" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="C25" s="15" t="s">
+      <c r="C25" s="24" t="s">
         <v>75</v>
       </c>
       <c r="D25" s="9" t="s">
@@ -2656,8 +2683,8 @@
       </c>
     </row>
     <row r="26" spans="2:12" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="B26" s="15"/>
-      <c r="C26" s="15"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
       <c r="D26" s="7" t="s">
         <v>79</v>
       </c>
@@ -2679,8 +2706,8 @@
       </c>
     </row>
     <row r="27" spans="2:12" ht="140.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
       <c r="D27" s="9" t="s">
         <v>82</v>
       </c>
@@ -2693,10 +2720,10 @@
       <c r="G27" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="I27" s="16" t="s">
+      <c r="I27" s="27" t="s">
         <v>21</v>
       </c>
       <c r="J27" s="10" t="s">
@@ -2707,22 +2734,22 @@
       </c>
     </row>
     <row r="28" spans="2:12" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
       <c r="D28" s="9" t="s">
         <v>86</v>
       </c>
       <c r="E28" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="F28" s="16" t="s">
+      <c r="F28" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="G28" s="16" t="s">
+      <c r="G28" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="H28" s="16"/>
-      <c r="I28" s="16"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
       <c r="J28" s="10" t="s">
         <v>150</v>
       </c>
@@ -2731,18 +2758,18 @@
       </c>
     </row>
     <row r="29" spans="2:12" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
+      <c r="B29" s="24"/>
+      <c r="C29" s="24"/>
       <c r="D29" s="9" t="s">
         <v>89</v>
       </c>
       <c r="E29" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="F29" s="16"/>
-      <c r="G29" s="16"/>
-      <c r="H29" s="16"/>
-      <c r="I29" s="16"/>
+      <c r="F29" s="27"/>
+      <c r="G29" s="27"/>
+      <c r="H29" s="27"/>
+      <c r="I29" s="27"/>
       <c r="J29" s="10" t="s">
         <v>158</v>
       </c>
@@ -2751,18 +2778,18 @@
       </c>
     </row>
     <row r="30" spans="2:12" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
+      <c r="B30" s="24"/>
+      <c r="C30" s="24"/>
       <c r="D30" s="9" t="s">
         <v>91</v>
       </c>
       <c r="E30" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="F30" s="16"/>
-      <c r="G30" s="16"/>
-      <c r="H30" s="16"/>
-      <c r="I30" s="16"/>
+      <c r="F30" s="27"/>
+      <c r="G30" s="27"/>
+      <c r="H30" s="27"/>
+      <c r="I30" s="27"/>
       <c r="J30" s="10" t="s">
         <v>163</v>
       </c>
@@ -2771,18 +2798,18 @@
       </c>
     </row>
     <row r="31" spans="2:12" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
       <c r="D31" s="9" t="s">
         <v>92</v>
       </c>
       <c r="E31" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="F31" s="16"/>
-      <c r="G31" s="16"/>
-      <c r="H31" s="16"/>
-      <c r="I31" s="16"/>
+      <c r="F31" s="27"/>
+      <c r="G31" s="27"/>
+      <c r="H31" s="27"/>
+      <c r="I31" s="27"/>
       <c r="J31" s="10" t="s">
         <v>149</v>
       </c>
@@ -2791,20 +2818,20 @@
       </c>
     </row>
     <row r="32" spans="2:12" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="24"/>
       <c r="D32" s="9" t="s">
         <v>93</v>
       </c>
       <c r="E32" s="12" t="s">
         <v>138</v>
       </c>
-      <c r="F32" s="16" t="s">
+      <c r="F32" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="G32" s="16"/>
-      <c r="H32" s="16"/>
-      <c r="I32" s="16"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
+      <c r="I32" s="27"/>
       <c r="J32" s="10" t="s">
         <v>156</v>
       </c>
@@ -2813,18 +2840,18 @@
       </c>
     </row>
     <row r="33" spans="2:12" ht="65.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="15"/>
-      <c r="C33" s="15"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="24"/>
       <c r="D33" s="9" t="s">
         <v>95</v>
       </c>
       <c r="E33" s="12" t="s">
         <v>139</v>
       </c>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
+      <c r="I33" s="27"/>
       <c r="J33" s="10" t="s">
         <v>148</v>
       </c>
@@ -2833,10 +2860,10 @@
       </c>
     </row>
     <row r="34" spans="2:12" ht="89.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="24" t="s">
         <v>96</v>
       </c>
-      <c r="C34" s="15" t="s">
+      <c r="C34" s="24" t="s">
         <v>97</v>
       </c>
       <c r="D34" s="9" t="s">
@@ -2845,16 +2872,16 @@
       <c r="E34" s="12" t="s">
         <v>140</v>
       </c>
-      <c r="F34" s="16" t="s">
+      <c r="F34" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="G34" s="16" t="s">
+      <c r="G34" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="H34" s="16" t="s">
+      <c r="H34" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="I34" s="16" t="s">
+      <c r="I34" s="27" t="s">
         <v>21</v>
       </c>
       <c r="J34" s="10" t="s">
@@ -2865,18 +2892,18 @@
       </c>
     </row>
     <row r="35" spans="2:12" ht="89.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="24"/>
       <c r="D35" s="9" t="s">
         <v>99</v>
       </c>
       <c r="E35" s="12" t="s">
         <v>141</v>
       </c>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
+      <c r="F35" s="27"/>
+      <c r="G35" s="27"/>
+      <c r="H35" s="27"/>
+      <c r="I35" s="27"/>
       <c r="J35" s="10" t="s">
         <v>175</v>
       </c>
@@ -2885,18 +2912,18 @@
       </c>
     </row>
     <row r="36" spans="2:12" ht="89.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="24"/>
       <c r="D36" s="9" t="s">
         <v>100</v>
       </c>
       <c r="E36" s="12" t="s">
         <v>142</v>
       </c>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
+      <c r="F36" s="27"/>
+      <c r="G36" s="27"/>
+      <c r="H36" s="27"/>
+      <c r="I36" s="27"/>
       <c r="J36" s="10" t="s">
         <v>182</v>
       </c>
@@ -2905,20 +2932,20 @@
       </c>
     </row>
     <row r="37" spans="2:12" ht="89.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="15"/>
-      <c r="C37" s="15"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
       <c r="D37" s="9" t="s">
         <v>101</v>
       </c>
       <c r="E37" s="12" t="s">
         <v>143</v>
       </c>
-      <c r="F37" s="16" t="s">
+      <c r="F37" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="G37" s="16"/>
-      <c r="H37" s="16"/>
-      <c r="I37" s="16"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
       <c r="J37" s="10" t="s">
         <v>174</v>
       </c>
@@ -2927,18 +2954,18 @@
       </c>
     </row>
     <row r="38" spans="2:12" ht="89.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
       <c r="D38" s="9" t="s">
         <v>103</v>
       </c>
       <c r="E38" s="12" t="s">
         <v>144</v>
       </c>
-      <c r="F38" s="16"/>
-      <c r="G38" s="16"/>
-      <c r="H38" s="16"/>
-      <c r="I38" s="16"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
       <c r="J38" s="10" t="s">
         <v>176</v>
       </c>
@@ -2947,22 +2974,22 @@
       </c>
     </row>
     <row r="39" spans="2:12" ht="89.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
       <c r="D39" s="9" t="s">
         <v>104</v>
       </c>
       <c r="E39" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="F39" s="16" t="s">
+      <c r="F39" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="G39" s="16" t="s">
+      <c r="G39" s="27" t="s">
         <v>146</v>
       </c>
-      <c r="H39" s="16"/>
-      <c r="I39" s="16"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
       <c r="J39" s="10" t="s">
         <v>192</v>
       </c>
@@ -2971,18 +2998,18 @@
       </c>
     </row>
     <row r="40" spans="2:12" ht="89.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
+      <c r="B40" s="24"/>
+      <c r="C40" s="24"/>
       <c r="D40" s="9" t="s">
         <v>106</v>
       </c>
       <c r="E40" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="F40" s="16"/>
-      <c r="G40" s="16"/>
-      <c r="H40" s="16"/>
-      <c r="I40" s="16"/>
+      <c r="F40" s="27"/>
+      <c r="G40" s="27"/>
+      <c r="H40" s="27"/>
+      <c r="I40" s="27"/>
       <c r="J40" s="10" t="s">
         <v>192</v>
       </c>
@@ -2991,18 +3018,18 @@
       </c>
     </row>
     <row r="41" spans="2:12" ht="89.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
+      <c r="B41" s="24"/>
+      <c r="C41" s="24"/>
       <c r="D41" s="9" t="s">
         <v>108</v>
       </c>
       <c r="E41" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="F41" s="16"/>
-      <c r="G41" s="16"/>
-      <c r="H41" s="16"/>
-      <c r="I41" s="16"/>
+      <c r="F41" s="27"/>
+      <c r="G41" s="27"/>
+      <c r="H41" s="27"/>
+      <c r="I41" s="27"/>
       <c r="J41" s="10" t="s">
         <v>207</v>
       </c>
@@ -3038,16 +3065,16 @@
       </c>
     </row>
     <row r="43" spans="2:12" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="24" t="s">
         <v>113</v>
       </c>
-      <c r="C43" s="15" t="s">
+      <c r="C43" s="24" t="s">
         <v>114</v>
       </c>
       <c r="D43" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="E43" s="17" t="s">
+      <c r="E43" s="25" t="s">
         <v>147</v>
       </c>
       <c r="F43" s="12"/>
@@ -3062,12 +3089,12 @@
       </c>
     </row>
     <row r="44" spans="2:12" ht="33.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
       <c r="D44" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="E44" s="17"/>
+      <c r="E44" s="25"/>
       <c r="F44" s="12"/>
       <c r="G44" s="12"/>
       <c r="H44" s="12"/>
@@ -3079,444 +3106,458 @@
         <v>162</v>
       </c>
     </row>
-    <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="11"/>
-      <c r="C45" s="11"/>
-      <c r="D45" s="24" t="s">
+    <row r="45" spans="2:12" ht="54" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="14"/>
+      <c r="C45" s="14"/>
+      <c r="D45" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="E45" s="15" t="s">
+        <v>215</v>
+      </c>
+      <c r="F45" s="15" t="s">
+        <v>216</v>
+      </c>
+      <c r="G45" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="H45" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I45" s="15" t="s">
+        <v>217</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="K45" s="10"/>
+    </row>
+    <row r="46" spans="2:12" x14ac:dyDescent="0.25">
+      <c r="B46" s="11"/>
+      <c r="C46" s="11"/>
+      <c r="D46" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="E45" s="24"/>
-      <c r="F45" s="24"/>
-      <c r="G45" s="24"/>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24"/>
-      <c r="J45" s="24"/>
-      <c r="K45" s="24"/>
-    </row>
-    <row r="46" spans="2:12" ht="98.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B46" s="15" t="s">
+      <c r="E46" s="26"/>
+      <c r="F46" s="26"/>
+      <c r="G46" s="26"/>
+      <c r="H46" s="26"/>
+      <c r="I46" s="26"/>
+      <c r="J46" s="26"/>
+      <c r="K46" s="26"/>
+    </row>
+    <row r="47" spans="2:12" ht="98.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="C46" s="15" t="s">
+      <c r="C47" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="D47" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="E46" s="18" t="s">
+      <c r="E47" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="F46" s="19" t="s">
+      <c r="F47" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="G46" s="18" t="s">
+      <c r="G47" s="16" t="s">
         <v>121</v>
       </c>
-      <c r="H46" s="20" t="s">
+      <c r="H47" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="I46" s="21" t="s">
+      <c r="I47" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="J46" s="22"/>
-      <c r="K46" s="23" t="s">
+      <c r="J47" s="20"/>
+      <c r="K47" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="47" spans="2:12" ht="79.7" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="18" t="s">
+    <row r="48" spans="2:12" ht="79.7" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="24"/>
+      <c r="C48" s="24"/>
+      <c r="D48" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="E47" s="18" t="s">
+      <c r="E48" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F47" s="19"/>
-      <c r="G47" s="18"/>
-      <c r="H47" s="20" t="s">
+      <c r="F48" s="17"/>
+      <c r="G48" s="16"/>
+      <c r="H48" s="18" t="s">
         <v>72</v>
       </c>
-      <c r="I47" s="21"/>
-      <c r="J47" s="22"/>
-      <c r="K47" s="23" t="s">
+      <c r="I48" s="19"/>
+      <c r="J48" s="20"/>
+      <c r="K48" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="48" spans="2:12" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="18" t="s">
+    <row r="49" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="D49" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="E48" s="18" t="s">
+      <c r="E49" s="16" t="s">
         <v>124</v>
       </c>
-      <c r="F48" s="19"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="21"/>
-      <c r="J48" s="22"/>
-      <c r="K48" s="23" t="s">
+      <c r="F49" s="17"/>
+      <c r="G49" s="16"/>
+      <c r="H49" s="16"/>
+      <c r="I49" s="19"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="49" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B49" s="15"/>
-      <c r="C49" s="15"/>
-      <c r="D49" s="18" t="s">
+    <row r="50" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
+      <c r="D50" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="E49" s="18" t="s">
+      <c r="E50" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F49" s="19"/>
-      <c r="G49" s="18"/>
-      <c r="H49" s="18"/>
-      <c r="I49" s="21"/>
-      <c r="J49" s="22"/>
-      <c r="K49" s="23" t="s">
+      <c r="F50" s="17"/>
+      <c r="G50" s="16"/>
+      <c r="H50" s="16"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="20"/>
+      <c r="K50" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="50" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B50" s="15"/>
-      <c r="C50" s="15"/>
-      <c r="D50" s="18" t="s">
+    <row r="51" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B51" s="24"/>
+      <c r="C51" s="24"/>
+      <c r="D51" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="E50" s="18" t="s">
+      <c r="E51" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F50" s="19"/>
-      <c r="G50" s="18"/>
-      <c r="H50" s="18"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="22"/>
-      <c r="K50" s="23" t="s">
+      <c r="F51" s="17"/>
+      <c r="G51" s="16"/>
+      <c r="H51" s="16"/>
+      <c r="I51" s="19"/>
+      <c r="J51" s="20"/>
+      <c r="K51" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="51" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="18" t="s">
+    <row r="52" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B52" s="24"/>
+      <c r="C52" s="24"/>
+      <c r="D52" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="E51" s="18" t="s">
+      <c r="E52" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F51" s="19"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="21"/>
-      <c r="J51" s="22"/>
-      <c r="K51" s="23" t="s">
+      <c r="F52" s="17"/>
+      <c r="G52" s="16"/>
+      <c r="H52" s="16"/>
+      <c r="I52" s="19"/>
+      <c r="J52" s="20"/>
+      <c r="K52" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="52" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B52" s="15"/>
-      <c r="C52" s="15"/>
-      <c r="D52" s="18" t="s">
+    <row r="53" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B53" s="24"/>
+      <c r="C53" s="24"/>
+      <c r="D53" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="E52" s="18" t="s">
+      <c r="E53" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F52" s="19"/>
-      <c r="G52" s="18"/>
-      <c r="H52" s="18"/>
-      <c r="I52" s="21"/>
-      <c r="J52" s="22"/>
-      <c r="K52" s="23" t="s">
+      <c r="F53" s="17"/>
+      <c r="G53" s="16"/>
+      <c r="H53" s="16"/>
+      <c r="I53" s="19"/>
+      <c r="J53" s="20"/>
+      <c r="K53" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="53" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="18" t="s">
+    <row r="54" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B54" s="24"/>
+      <c r="C54" s="24"/>
+      <c r="D54" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="E53" s="18" t="s">
+      <c r="E54" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F53" s="19"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="21"/>
-      <c r="J53" s="22"/>
-      <c r="K53" s="23" t="s">
+      <c r="F54" s="17"/>
+      <c r="G54" s="16"/>
+      <c r="H54" s="16"/>
+      <c r="I54" s="19"/>
+      <c r="J54" s="20"/>
+      <c r="K54" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="54" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="18" t="s">
+    <row r="55" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B55" s="24"/>
+      <c r="C55" s="24"/>
+      <c r="D55" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="E54" s="18" t="s">
+      <c r="E55" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F54" s="19"/>
-      <c r="G54" s="18"/>
-      <c r="H54" s="18"/>
-      <c r="I54" s="21"/>
-      <c r="J54" s="22"/>
-      <c r="K54" s="23" t="s">
+      <c r="F55" s="17"/>
+      <c r="G55" s="16"/>
+      <c r="H55" s="16"/>
+      <c r="I55" s="19"/>
+      <c r="J55" s="20"/>
+      <c r="K55" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="55" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="18" t="s">
+    <row r="56" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B56" s="24"/>
+      <c r="C56" s="24"/>
+      <c r="D56" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="E55" s="18" t="s">
+      <c r="E56" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F55" s="19"/>
-      <c r="G55" s="18"/>
-      <c r="H55" s="18"/>
-      <c r="I55" s="21"/>
-      <c r="J55" s="22"/>
-      <c r="K55" s="23" t="s">
+      <c r="F56" s="17"/>
+      <c r="G56" s="16"/>
+      <c r="H56" s="16"/>
+      <c r="I56" s="19"/>
+      <c r="J56" s="20"/>
+      <c r="K56" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="56" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B56" s="15"/>
-      <c r="C56" s="15"/>
-      <c r="D56" s="18" t="s">
+    <row r="57" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B57" s="24"/>
+      <c r="C57" s="24"/>
+      <c r="D57" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="E56" s="18" t="s">
+      <c r="E57" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F56" s="19"/>
-      <c r="G56" s="18"/>
-      <c r="H56" s="18"/>
-      <c r="I56" s="21"/>
-      <c r="J56" s="22"/>
-      <c r="K56" s="23" t="s">
+      <c r="F57" s="17"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
+      <c r="I57" s="19"/>
+      <c r="J57" s="20"/>
+      <c r="K57" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="57" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="18" t="s">
+    <row r="58" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B58" s="24"/>
+      <c r="C58" s="24"/>
+      <c r="D58" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E57" s="18" t="s">
+      <c r="E58" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F57" s="19"/>
-      <c r="G57" s="18"/>
-      <c r="H57" s="18"/>
-      <c r="I57" s="21"/>
-      <c r="J57" s="22"/>
-      <c r="K57" s="23" t="s">
+      <c r="F58" s="17"/>
+      <c r="G58" s="16"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="19"/>
+      <c r="J58" s="20"/>
+      <c r="K58" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="58" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B58" s="15"/>
-      <c r="C58" s="15"/>
-      <c r="D58" s="18" t="s">
+    <row r="59" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B59" s="24"/>
+      <c r="C59" s="24"/>
+      <c r="D59" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E58" s="18" t="s">
+      <c r="E59" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F58" s="19"/>
-      <c r="G58" s="18"/>
-      <c r="H58" s="18"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="22"/>
-      <c r="K58" s="23" t="s">
+      <c r="F59" s="17"/>
+      <c r="G59" s="16"/>
+      <c r="H59" s="16"/>
+      <c r="I59" s="19"/>
+      <c r="J59" s="20"/>
+      <c r="K59" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="59" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="18" t="s">
+    <row r="60" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B60" s="24"/>
+      <c r="C60" s="24"/>
+      <c r="D60" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="E59" s="18" t="s">
+      <c r="E60" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="F59" s="19"/>
-      <c r="G59" s="18"/>
-      <c r="H59" s="18"/>
-      <c r="I59" s="21"/>
-      <c r="J59" s="22"/>
-      <c r="K59" s="23" t="s">
+      <c r="F60" s="17"/>
+      <c r="G60" s="16"/>
+      <c r="H60" s="16"/>
+      <c r="I60" s="19"/>
+      <c r="J60" s="20"/>
+      <c r="K60" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="60" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B60" s="15"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="18" t="s">
+    <row r="61" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B61" s="24"/>
+      <c r="C61" s="24"/>
+      <c r="D61" s="16" t="s">
         <v>19</v>
       </c>
-      <c r="E60" s="18" t="s">
+      <c r="E61" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F60" s="19"/>
-      <c r="G60" s="18"/>
-      <c r="H60" s="18"/>
-      <c r="I60" s="21"/>
-      <c r="J60" s="22"/>
-      <c r="K60" s="23" t="s">
+      <c r="F61" s="17"/>
+      <c r="G61" s="16"/>
+      <c r="H61" s="16"/>
+      <c r="I61" s="19"/>
+      <c r="J61" s="20"/>
+      <c r="K61" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="61" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B61" s="15"/>
-      <c r="C61" s="15"/>
-      <c r="D61" s="18" t="s">
+    <row r="62" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B62" s="24"/>
+      <c r="C62" s="24"/>
+      <c r="D62" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="E61" s="18" t="s">
+      <c r="E62" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F61" s="19"/>
-      <c r="G61" s="18"/>
-      <c r="H61" s="18"/>
-      <c r="I61" s="21"/>
-      <c r="J61" s="22"/>
-      <c r="K61" s="23" t="s">
+      <c r="F62" s="17"/>
+      <c r="G62" s="16"/>
+      <c r="H62" s="16"/>
+      <c r="I62" s="19"/>
+      <c r="J62" s="20"/>
+      <c r="K62" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="62" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B62" s="15"/>
-      <c r="C62" s="15"/>
-      <c r="D62" s="18" t="s">
+    <row r="63" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B63" s="24"/>
+      <c r="C63" s="24"/>
+      <c r="D63" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="E62" s="18" t="s">
+      <c r="E63" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F62" s="19"/>
-      <c r="G62" s="18"/>
-      <c r="H62" s="18"/>
-      <c r="I62" s="21"/>
-      <c r="J62" s="22"/>
-      <c r="K62" s="23" t="s">
+      <c r="F63" s="17"/>
+      <c r="G63" s="16"/>
+      <c r="H63" s="16"/>
+      <c r="I63" s="19"/>
+      <c r="J63" s="20"/>
+      <c r="K63" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="63" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B63" s="15"/>
-      <c r="C63" s="15"/>
-      <c r="D63" s="18" t="s">
+    <row r="64" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B64" s="24"/>
+      <c r="C64" s="24"/>
+      <c r="D64" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="E63" s="18" t="s">
+      <c r="E64" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F63" s="19"/>
-      <c r="G63" s="18"/>
-      <c r="H63" s="18"/>
-      <c r="I63" s="21"/>
-      <c r="J63" s="22"/>
-      <c r="K63" s="23" t="s">
+      <c r="F64" s="17"/>
+      <c r="G64" s="16"/>
+      <c r="H64" s="16"/>
+      <c r="I64" s="19"/>
+      <c r="J64" s="20"/>
+      <c r="K64" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="64" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B64" s="15"/>
-      <c r="C64" s="15"/>
-      <c r="D64" s="18" t="s">
+    <row r="65" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B65" s="24"/>
+      <c r="C65" s="24"/>
+      <c r="D65" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="E64" s="18" t="s">
+      <c r="E65" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F64" s="19"/>
-      <c r="G64" s="18"/>
-      <c r="H64" s="18"/>
-      <c r="I64" s="21"/>
-      <c r="J64" s="22"/>
-      <c r="K64" s="23" t="s">
+      <c r="F65" s="17"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
+      <c r="I65" s="19"/>
+      <c r="J65" s="20"/>
+      <c r="K65" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="65" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B65" s="15"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="18" t="s">
+    <row r="66" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B66" s="24"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="E65" s="18" t="s">
+      <c r="E66" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F65" s="19"/>
-      <c r="G65" s="18"/>
-      <c r="H65" s="18"/>
-      <c r="I65" s="21"/>
-      <c r="J65" s="22"/>
-      <c r="K65" s="23" t="s">
+      <c r="F66" s="17"/>
+      <c r="G66" s="16"/>
+      <c r="H66" s="16"/>
+      <c r="I66" s="19"/>
+      <c r="J66" s="20"/>
+      <c r="K66" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="66" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B66" s="15"/>
-      <c r="C66" s="15"/>
-      <c r="D66" s="18" t="s">
+    <row r="67" spans="2:11" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B67" s="24"/>
+      <c r="C67" s="24"/>
+      <c r="D67" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="E66" s="18" t="s">
+      <c r="E67" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="F66" s="19"/>
-      <c r="G66" s="18"/>
-      <c r="H66" s="18"/>
-      <c r="I66" s="21"/>
-      <c r="J66" s="22"/>
-      <c r="K66" s="23" t="s">
+      <c r="F67" s="17"/>
+      <c r="G67" s="16"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="19"/>
+      <c r="J67" s="20"/>
+      <c r="K67" s="21" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="67" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B67" s="14" t="s">
+    <row r="68" spans="2:11" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="23" t="s">
         <v>127</v>
       </c>
-      <c r="C67" s="14"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="14"/>
-      <c r="F67" s="14"/>
-      <c r="G67" s="14"/>
-      <c r="H67" s="14"/>
-      <c r="I67" s="14"/>
-      <c r="J67" s="14"/>
+      <c r="C68" s="23"/>
+      <c r="D68" s="23"/>
+      <c r="E68" s="23"/>
+      <c r="F68" s="23"/>
+      <c r="G68" s="23"/>
+      <c r="H68" s="23"/>
+      <c r="I68" s="23"/>
+      <c r="J68" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="30">
-    <mergeCell ref="B67:J67"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="E43:E44"/>
-    <mergeCell ref="D45:K45"/>
-    <mergeCell ref="B46:B66"/>
-    <mergeCell ref="C46:C66"/>
-    <mergeCell ref="B34:B41"/>
-    <mergeCell ref="C34:C41"/>
-    <mergeCell ref="F34:F36"/>
-    <mergeCell ref="G34:G38"/>
-    <mergeCell ref="H34:H41"/>
-    <mergeCell ref="I34:I41"/>
-    <mergeCell ref="F37:F38"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="G39:G41"/>
-    <mergeCell ref="I14:I23"/>
+    <mergeCell ref="B3:B13"/>
+    <mergeCell ref="C3:C13"/>
+    <mergeCell ref="B14:B24"/>
+    <mergeCell ref="C14:C24"/>
+    <mergeCell ref="G14:G23"/>
     <mergeCell ref="B25:B33"/>
     <mergeCell ref="C25:C33"/>
     <mergeCell ref="H27:H33"/>
@@ -3524,14 +3565,27 @@
     <mergeCell ref="F28:F31"/>
     <mergeCell ref="G28:G33"/>
     <mergeCell ref="F32:F33"/>
-    <mergeCell ref="B3:B13"/>
-    <mergeCell ref="C3:C13"/>
-    <mergeCell ref="B14:B24"/>
-    <mergeCell ref="C14:C24"/>
-    <mergeCell ref="G14:G23"/>
+    <mergeCell ref="I34:I41"/>
+    <mergeCell ref="F37:F38"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="I14:I23"/>
     <mergeCell ref="H14:H23"/>
+    <mergeCell ref="B34:B41"/>
+    <mergeCell ref="C34:C41"/>
+    <mergeCell ref="F34:F36"/>
+    <mergeCell ref="G34:G38"/>
+    <mergeCell ref="H34:H41"/>
+    <mergeCell ref="B68:J68"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="E43:E44"/>
+    <mergeCell ref="D46:K46"/>
+    <mergeCell ref="B47:B67"/>
+    <mergeCell ref="C47:C67"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Complete cross-ref review against coverage model
Signed-off-by: Mike Thompson <mike@openhwgroup.org>
</commit_message>
<xml_diff>
--- a/verif/CV32E40P/SimulationVerificationPlan/base_instruction_set/CV32E40P_RV32I_Base_Instructions.xlsx
+++ b/verif/CV32E40P/SimulationVerificationPlan/base_instruction_set/CV32E40P_RV32I_Base_Instructions.xlsx
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="229">
   <si>
     <t xml:space="preserve">Requirement Location</t>
   </si>
@@ -1564,6 +1564,96 @@
   </si>
   <si>
     <t xml:space="preserve">Normal FENCE with pred==0 | succ==0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chapter 9.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSR Instructions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSRRW</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csrrw rd, csr, rs1
+tmp = CSR[csr];
+CSR[csr] = x[rs1];
+x[rd] = tmp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercise instruction using all legal destination CSRs, including x0.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Step-and-compare with ISS.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test case (Compliance).
+Functional coverage of verification goals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uvme_rv32isa_covg.sv.csrrw_cg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSRRS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csrrs rd, csr, rs1
+tmp = CSR[csr];
+CSR[csr] = tmp | x[rs1];
+x[rd] = tmp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uvme_rv32isa_covg.sv.csrs_cg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSRRC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csrrc rd, csr, rs1
+tmp = CSR[csr];
+CSR[csr] = tmp &amp; ~x[rs1];
+x[rd] = tmp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uvme_rv32isa_covg.sv.csrrc_cg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSRRWI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csrrwi rd, csr, zimm[4:0]
+x[rd] = CSR[csr];
+CSR[csr] = zimm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exercise instruction using all legal destination CSRs, including x0.  Cover range of immediate values.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uvme_rv32isa_covg.sv.csrrwi_cg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSRRSI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csrrsi rd, csr, zimm[4:0]
+tmp = CSR[csr];
+CSR[csr] = tmp | zimm;
+x[rd] = tmp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uvme_rv32isa_covg.sv.csrrsi_cg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CSRRCI</t>
+  </si>
+  <si>
+    <t xml:space="preserve">csrrci rd, csr, zimm[4:0]
+tmp = CSR[csr];
+CSR[csr] = tmp &amp; ~zimm;
+x[rd] = tmp;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uvme_rv32isa_covg.sv.csrrci_cg</t>
   </si>
   <si>
     <t xml:space="preserve"> -------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------- END -----------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------------</t>
@@ -1576,7 +1666,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1638,6 +1728,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="7">
@@ -1712,7 +1808,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1805,6 +1901,18 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1890,29 +1998,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B1:L68"/>
+  <dimension ref="B1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="17.01953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="1.58"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="2" min="2" style="2" width="13.7"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="3" min="3" style="2" width="20.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="13.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="20.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="8.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="51.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="41.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="34.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="51.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="41.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="34.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="16.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="35.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="36.26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="2" width="66"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1015" min="12" style="2" width="17"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="1016" style="2" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1017" min="1016" style="2" width="9.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1018" style="1" width="8.71"/>
   </cols>
   <sheetData>
@@ -2926,7 +3034,7 @@
       </c>
       <c r="K41" s="8"/>
     </row>
-    <row r="42" customFormat="false" ht="33.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="42.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B42" s="7" t="s">
         <v>177</v>
       </c>
@@ -3029,7 +3137,7 @@
       <c r="J46" s="16"/>
       <c r="K46" s="16"/>
     </row>
-    <row r="47" customFormat="false" ht="98.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="98.1" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B47" s="10" t="s">
         <v>194</v>
       </c>
@@ -3059,7 +3167,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="79.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="79.7" hidden="true" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="10"/>
       <c r="C48" s="10"/>
       <c r="D48" s="17" t="s">
@@ -3079,7 +3187,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="10"/>
       <c r="C49" s="10"/>
       <c r="D49" s="17" t="s">
@@ -3097,7 +3205,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="10"/>
       <c r="C50" s="10"/>
       <c r="D50" s="17" t="s">
@@ -3115,7 +3223,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="10"/>
       <c r="C51" s="10"/>
       <c r="D51" s="17" t="s">
@@ -3133,7 +3241,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
       <c r="D52" s="17" t="s">
@@ -3151,7 +3259,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="10"/>
       <c r="C53" s="10"/>
       <c r="D53" s="17" t="s">
@@ -3169,7 +3277,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="10"/>
       <c r="C54" s="10"/>
       <c r="D54" s="17" t="s">
@@ -3187,7 +3295,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="10"/>
       <c r="C55" s="10"/>
       <c r="D55" s="17" t="s">
@@ -3205,7 +3313,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="10"/>
       <c r="C56" s="10"/>
       <c r="D56" s="17" t="s">
@@ -3223,7 +3331,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B57" s="10"/>
       <c r="C57" s="10"/>
       <c r="D57" s="17" t="s">
@@ -3241,7 +3349,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B58" s="10"/>
       <c r="C58" s="10"/>
       <c r="D58" s="17" t="s">
@@ -3259,7 +3367,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B59" s="10"/>
       <c r="C59" s="10"/>
       <c r="D59" s="17" t="s">
@@ -3277,7 +3385,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B60" s="10"/>
       <c r="C60" s="10"/>
       <c r="D60" s="17" t="s">
@@ -3295,7 +3403,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="61" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B61" s="10"/>
       <c r="C61" s="10"/>
       <c r="D61" s="17" t="s">
@@ -3313,7 +3421,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B62" s="10"/>
       <c r="C62" s="10"/>
       <c r="D62" s="17" t="s">
@@ -3331,7 +3439,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="63" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="63" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B63" s="10"/>
       <c r="C63" s="10"/>
       <c r="D63" s="17" t="s">
@@ -3349,7 +3457,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B64" s="10"/>
       <c r="C64" s="10"/>
       <c r="D64" s="17" t="s">
@@ -3367,7 +3475,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B65" s="10"/>
       <c r="C65" s="10"/>
       <c r="D65" s="17" t="s">
@@ -3385,7 +3493,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="10"/>
       <c r="C66" s="10"/>
       <c r="D66" s="17" t="s">
@@ -3403,7 +3511,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="31.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" customFormat="false" ht="31.5" hidden="true" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B67" s="10"/>
       <c r="C67" s="10"/>
       <c r="D67" s="17" t="s">
@@ -3421,21 +3529,147 @@
         <v>200</v>
       </c>
     </row>
-    <row r="68" s="23" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="24" t="s">
+    <row r="68" customFormat="false" ht="61.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B68" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="C68" s="24"/>
-      <c r="D68" s="24"/>
-      <c r="E68" s="24"/>
-      <c r="F68" s="24"/>
-      <c r="G68" s="24"/>
-      <c r="H68" s="24"/>
-      <c r="I68" s="24"/>
-      <c r="J68" s="24"/>
-    </row>
+      <c r="C68" s="10" t="s">
+        <v>205</v>
+      </c>
+      <c r="D68" s="7" t="s">
+        <v>206</v>
+      </c>
+      <c r="E68" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="F68" s="23" t="s">
+        <v>208</v>
+      </c>
+      <c r="G68" s="24" t="s">
+        <v>209</v>
+      </c>
+      <c r="H68" s="24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I68" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="J68" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="K68" s="7"/>
+    </row>
+    <row r="69" customFormat="false" ht="62.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B69" s="10"/>
+      <c r="C69" s="10"/>
+      <c r="D69" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E69" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="F69" s="23"/>
+      <c r="G69" s="24"/>
+      <c r="H69" s="24"/>
+      <c r="I69" s="24"/>
+      <c r="J69" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="K69" s="7"/>
+    </row>
+    <row r="70" customFormat="false" ht="62.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B70" s="10"/>
+      <c r="C70" s="10"/>
+      <c r="D70" s="7" t="s">
+        <v>215</v>
+      </c>
+      <c r="E70" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="F70" s="23"/>
+      <c r="G70" s="24"/>
+      <c r="H70" s="24"/>
+      <c r="I70" s="24"/>
+      <c r="J70" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="K70" s="7"/>
+    </row>
+    <row r="71" customFormat="false" ht="50.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B71" s="10"/>
+      <c r="C71" s="10"/>
+      <c r="D71" s="7" t="s">
+        <v>218</v>
+      </c>
+      <c r="E71" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="F71" s="23" t="s">
+        <v>220</v>
+      </c>
+      <c r="G71" s="24"/>
+      <c r="H71" s="24"/>
+      <c r="I71" s="24"/>
+      <c r="J71" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="K71" s="7"/>
+    </row>
+    <row r="72" customFormat="false" ht="62.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B72" s="10"/>
+      <c r="C72" s="10"/>
+      <c r="D72" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E72" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="F72" s="23"/>
+      <c r="G72" s="24"/>
+      <c r="H72" s="24"/>
+      <c r="I72" s="24"/>
+      <c r="J72" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="K72" s="7"/>
+    </row>
+    <row r="73" customFormat="false" ht="62.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B73" s="10"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="E73" s="7" t="s">
+        <v>226</v>
+      </c>
+      <c r="F73" s="23"/>
+      <c r="G73" s="24"/>
+      <c r="H73" s="24"/>
+      <c r="I73" s="24"/>
+      <c r="J73" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="K73" s="7"/>
+    </row>
+    <row r="74" s="26" customFormat="true" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B74" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="C74" s="27"/>
+      <c r="D74" s="27"/>
+      <c r="E74" s="27"/>
+      <c r="F74" s="27"/>
+      <c r="G74" s="27"/>
+      <c r="H74" s="27"/>
+      <c r="I74" s="27"/>
+      <c r="J74" s="27"/>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="37">
     <mergeCell ref="B3:B13"/>
     <mergeCell ref="C3:C13"/>
     <mergeCell ref="B14:B24"/>
@@ -3465,7 +3699,14 @@
     <mergeCell ref="D46:K46"/>
     <mergeCell ref="B47:B67"/>
     <mergeCell ref="C47:C67"/>
-    <mergeCell ref="B68:J68"/>
+    <mergeCell ref="B68:B73"/>
+    <mergeCell ref="C68:C73"/>
+    <mergeCell ref="F68:F70"/>
+    <mergeCell ref="G68:G73"/>
+    <mergeCell ref="H68:H73"/>
+    <mergeCell ref="I68:I73"/>
+    <mergeCell ref="F71:F73"/>
+    <mergeCell ref="B74:J74"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>